<commit_message>
PC Value Tracker: Add V3 design docs, classification rules, and new reporting scripts
</commit_message>
<xml_diff>
--- a/PC_Value_Tracker/output/monthly/Monthly_Report_2025-10.xlsx
+++ b/PC_Value_Tracker/output/monthly/Monthly_Report_2025-10.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-24 19:42</t>
+          <t>2026-01-25 07:04</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>BY STREAM</t>
         </is>
@@ -496,13 +496,13 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Day-to-Day</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -512,39 +512,39 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Diagnostic</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>BY SYSTEM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BY SYSTEM</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Alarm</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -552,19 +552,19 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Alarm</t>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SIS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SIS</t>
+          <t>DCS</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -574,228 +574,198 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DCS</t>
+          <t>HMI</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HMI</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Network</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>BY COMPLEXITY</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BY COMPLEXITY</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>High</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>BY BUSINESS IMPACT</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BY BUSINESS IMPACT</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Compliance</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>4</v>
-      </c>
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Safety</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>2</v>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>BY RESOLUTION</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BY RESOLUTION</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Escalated</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Handed Off</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Workaround</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Escalated</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Handed Off</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Workaround</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -873,7 +843,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -883,12 +853,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -920,12 +890,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
@@ -957,12 +927,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
@@ -984,7 +954,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Diagnostic</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -999,7 +969,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1021,7 +991,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Diagnostic</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1036,7 +1006,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1028,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1068,7 +1038,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1110,7 +1080,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1112,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1169,7 +1139,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1184,7 +1154,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1191,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1228,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1290,12 +1260,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1327,12 +1297,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1339,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1376,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
@@ -1438,12 +1408,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1450,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1550,27 +1520,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Experion/TPS</t>
+          <t>Historian</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FW: LARINT01 - Cannot create scheduled task: Documented export cadences (EXP/TPS) and reiterated sch</t>
+          <t>RE: Marathon | St Paul | Pre-Onsite Visit: Clarified PI vs. PHD architecture and suggested staging P</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1582,17 +1552,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DCS</t>
+          <t>Alarm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cleaned ghost references on ESVT3 for Butamer tags</t>
+          <t>Deployed patched SyncDriver DLL for Dynamo fix</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1607,14 +1577,14 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1624,7 +1594,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Deployed patched SyncDriver DLL for Dynamo fix</t>
+          <t>Workaround for ACM PT DESC update via Station F12</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1634,19 +1604,19 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Workaround</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1656,7 +1626,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Workaround for ACM PT DESC update via Station F12</t>
+          <t>Clarified alarm governance L4/L3 for APO/ACM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1666,29 +1636,29 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Workaround</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Alarm</t>
+          <t>Integrity</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Clarified alarm governance L4/L3 for APO/ACM</t>
+          <t>Created scheduled task to move EPKS files on LARINT01</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1708,39 +1678,19 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-10-30</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Integrity</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Created scheduled task to move EPKS files on LARINT01</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Efficiency</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === DAY-TO-DAY ===</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1750,61 +1700,81 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === DAY-TO-DAY ===</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Resolution</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>SIS/Triconex</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>RE: HCU TMR Alarm: Referenced prior EDM training for pulling system faults; recommended shadowing fo</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Complexity</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Resolution</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Impact</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Historian</t>
+          <t>SIS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RE: Marathon | St Paul | Pre-Onsite Visit: Clarified PI vs. PHD architecture and suggested staging P</t>
+          <t>Guided use of EDM for fault logs and training</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1814,76 +1784,76 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SIS/Triconex</t>
+          <t>Turbine</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RE: HCU TMR Alarm: Referenced prior EDM training for pulling system faults; recommended shadowing fo</t>
+          <t>Investigated DWATT TOO LOW and suggested GE ticket</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Escalated</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SIS</t>
+          <t>DCS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Guided use of EDM for fault logs and training</t>
+          <t>Assessed loss of steam extraction control on STG#2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Handed Off</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1895,140 +1865,140 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>HMI</t>
+          <t>Experion/TPS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Identified need for Vartech HMI driver CD-ROM</t>
+          <t>FW: LARINT01 - Cannot create scheduled task: Documented export cadences (EXP/TPS) and reiterated sch</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>High</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GE/Woodward/Bently</t>
+          <t>HMI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>WCC 92 Power Distribution Card Failure: Initiated follow-up on power distribution card incident; not</t>
+          <t>Identified need for Vartech HMI driver CD-ROM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>GE/Woodward/Bently</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Confirmed KepServerEX licenses for Modbus Master</t>
+          <t>WCC 92 Power Distribution Card Failure: Initiated follow-up on power distribution card incident; not</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Alarm</t>
+          <t>DCS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Requested failover of ESVT3 after collection stopped</t>
+          <t>Cleaned ghost references on ESVT3 for Butamer tags</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SIS</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Advised on simulating Safety Manager comms</t>
+          <t>Confirmed KepServerEX licenses for Modbus Master</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2038,170 +2008,118 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Alarm</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Requested failover of ESVT3 after collection stopped</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>HMI</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Resolved by adjusting dewpoint setpoints on HMIs</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Fixed</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SIS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Advised on simulating Safety Manager comms</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === DIAGNOSTIC ===</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>HMI</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Resolved by adjusting dewpoint setpoints on HMIs</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Complexity</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Resolution</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Impact</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-10-13</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Turbine</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Investigated DWATT TOO LOW and suggested GE ticket</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Escalated</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-10-14</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>DCS</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Assessed loss of steam extraction control on STG#2</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Handed Off</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2431,7 +2349,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Diagnostic</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2458,7 +2376,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2485,7 +2403,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2629,7 +2547,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2656,7 +2574,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Diagnostic</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">

</xml_diff>